<commit_message>
Add IASP images and update emotion regulation files
Added a large set of IASP images for the emotion regulation experiment, updated block association and intro loop files, replaced main trial CSV with separate neutral, practice, and unpleasant trial files, and updated PsychoPy experiment files to reflect these changes.
</commit_message>
<xml_diff>
--- a/docs/emotion_regulation_block_association.xlsx
+++ b/docs/emotion_regulation_block_association.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29602"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\clini\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\neuroflare-experiments\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90F396ED-BC7E-4D4A-A4F1-A7F8FEED74C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE02CB27-5047-4E88-A842-4A10E8DC5853}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="135" yWindow="0" windowWidth="26430" windowHeight="15480" xr2:uid="{B6D0782D-5CF3-428D-9361-9D827529FAEF}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B6D0782D-5CF3-428D-9361-9D827529FAEF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="109">
   <si>
     <t>BLOCK 1</t>
   </si>
@@ -60,9 +60,6 @@
     <t>practice</t>
   </si>
   <si>
-    <t>Currently, they are filled with placeholders</t>
-  </si>
-  <si>
     <t>spider</t>
   </si>
   <si>
@@ -364,13 +361,16 @@
   </si>
   <si>
     <t>꽁초</t>
+  </si>
+  <si>
+    <t>Practice</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -387,49 +387,12 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="13">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -443,28 +406,163 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -799,746 +897,777 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4251DC50-3AF3-42DE-A162-0BBAD3E34EA2}">
-  <dimension ref="A1:O41"/>
+  <dimension ref="A1:I41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="4" width="8.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15.75" thickBot="1">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="N1" t="s">
-        <v>5</v>
-      </c>
-      <c r="O1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15">
-      <c r="A2">
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
         <v>1019</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="4">
         <v>1022</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="4">
         <v>1026</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="6">
         <v>1030</v>
       </c>
-      <c r="F2" t="s">
-        <v>7</v>
-      </c>
-      <c r="N2">
+      <c r="F2" s="14">
         <v>2272</v>
       </c>
-      <c r="O2">
+      <c r="G2" s="12">
         <v>1205</v>
       </c>
     </row>
-    <row r="3" spans="1:15">
-      <c r="A3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="5">
         <v>1040</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="4">
         <v>1050</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="4">
         <v>1051</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="6">
         <v>1052</v>
       </c>
-      <c r="N3">
+      <c r="F3" s="14">
         <v>2383</v>
       </c>
-      <c r="O3">
+      <c r="G3" s="6">
         <v>3103</v>
       </c>
     </row>
-    <row r="4" spans="1:15">
-      <c r="A4">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="5">
         <v>1070</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="4">
         <v>1080</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="4">
         <v>1090</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="6">
         <v>1101</v>
       </c>
-      <c r="N4">
+      <c r="F4" s="14">
         <v>2393</v>
       </c>
-      <c r="O4">
+      <c r="G4" s="6">
         <v>3180</v>
       </c>
     </row>
-    <row r="5" spans="1:15">
-      <c r="A5">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="5">
         <v>1110</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="4">
         <v>1111</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="4">
         <v>1114</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="6">
         <v>1200</v>
       </c>
-      <c r="N5">
+      <c r="F5" s="14">
         <v>2396</v>
       </c>
-      <c r="O5">
+      <c r="G5" s="6">
         <v>3213</v>
       </c>
     </row>
-    <row r="6" spans="1:15">
-      <c r="A6">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="5">
         <v>1201</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="4">
         <v>1274</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="4">
         <v>1275</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="6">
         <v>1300</v>
       </c>
-      <c r="N6">
+      <c r="F6" s="14">
         <v>2397</v>
       </c>
-      <c r="O6">
+      <c r="G6" s="6">
         <v>3220</v>
       </c>
     </row>
-    <row r="7" spans="1:15">
-      <c r="A7">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="5">
         <v>1321</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="4">
         <v>1302</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="4">
         <v>1301</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="6">
         <v>1932</v>
       </c>
-      <c r="N7">
+      <c r="F7" s="14">
         <v>2435</v>
       </c>
-      <c r="O7">
+      <c r="G7" s="6">
         <v>3280</v>
       </c>
     </row>
-    <row r="8" spans="1:15">
-      <c r="A8">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="5">
         <v>2130</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="4">
         <v>2120</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="4">
         <v>2095</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="6">
         <v>2205</v>
       </c>
-      <c r="N8">
+      <c r="F8" s="14">
         <v>2480</v>
       </c>
-      <c r="O8">
+      <c r="G8" s="6">
         <v>5970</v>
       </c>
     </row>
-    <row r="9" spans="1:15">
-      <c r="A9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="5">
         <v>2691</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="4">
         <v>2683</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="4">
         <v>2220</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="6">
         <v>2692</v>
       </c>
-      <c r="N9">
+      <c r="F9" s="14">
         <v>2514</v>
       </c>
-      <c r="O9">
+      <c r="G9" s="3">
         <v>6190</v>
       </c>
     </row>
-    <row r="10" spans="1:15">
-      <c r="A10">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="5">
         <v>2700</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="4">
         <v>2695</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="4">
         <v>2694</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="6">
         <v>2703</v>
       </c>
-      <c r="N10">
+      <c r="F10" s="14">
         <v>2518</v>
       </c>
-    </row>
-    <row r="11" spans="1:15">
-      <c r="A11">
+      <c r="G10" s="4"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="5">
         <v>2751</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="4">
         <v>2705</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="4">
         <v>2704</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="6">
         <v>2795</v>
       </c>
-      <c r="N11">
+      <c r="F11" s="14">
         <v>2575</v>
       </c>
-    </row>
-    <row r="12" spans="1:15">
-      <c r="A12">
+      <c r="G11" s="4"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="5">
         <v>2811</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="4">
         <v>2800</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="4">
         <v>2799</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="6">
         <v>2900</v>
       </c>
-      <c r="N12">
+      <c r="F12" s="14">
         <v>2580</v>
       </c>
-    </row>
-    <row r="13" spans="1:15">
-      <c r="A13">
+      <c r="G12" s="4"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="5">
         <v>3016</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="4">
         <v>3005</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="4">
         <v>3001</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="6">
         <v>3030</v>
       </c>
-      <c r="N13">
+      <c r="F13" s="14">
         <v>2593</v>
       </c>
-    </row>
-    <row r="14" spans="1:15">
-      <c r="A14">
+      <c r="G13" s="4"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="5">
         <v>3215</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="4">
         <v>3181</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="4">
         <v>3110</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="6">
         <v>3225</v>
       </c>
-      <c r="N14">
+      <c r="F14" s="14">
         <v>2594</v>
       </c>
-    </row>
-    <row r="15" spans="1:15">
-      <c r="A15">
+      <c r="G14" s="4"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="5">
         <v>3301</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="4">
         <v>3300</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="4">
         <v>3230</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="6">
         <v>3500</v>
       </c>
-      <c r="N15">
+      <c r="F15" s="14">
         <v>2870</v>
       </c>
-    </row>
-    <row r="16" spans="1:15">
-      <c r="A16">
+      <c r="G15" s="4"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="5">
         <v>5920</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="4">
         <v>4621</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="4">
         <v>3530</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="6">
         <v>5950</v>
       </c>
-      <c r="N16">
+      <c r="F16" s="14">
         <v>2880</v>
       </c>
-    </row>
-    <row r="17" spans="1:14">
-      <c r="A17">
+      <c r="G16" s="4"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="5">
         <v>6010</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="4">
         <v>5973</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="4">
         <v>5971</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="6">
         <v>6200</v>
       </c>
-      <c r="N17">
+      <c r="F17" s="14">
         <v>2980</v>
       </c>
-    </row>
-    <row r="18" spans="1:14">
-      <c r="A18">
+      <c r="G17" s="4"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="5">
         <v>6242</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="4">
         <v>6241</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="4">
         <v>6212</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="6">
         <v>6243</v>
       </c>
-      <c r="N18">
+      <c r="F18" s="14">
         <v>5395</v>
       </c>
-    </row>
-    <row r="19" spans="1:14">
-      <c r="A19">
+      <c r="G18" s="4"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="5">
         <v>6311</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="4">
         <v>6260</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="4">
         <v>6250</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="6">
         <v>6312</v>
       </c>
-      <c r="N19">
+      <c r="F19" s="14">
         <v>5455</v>
       </c>
-    </row>
-    <row r="20" spans="1:14">
-      <c r="A20">
+      <c r="G19" s="4"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="5">
         <v>6370</v>
       </c>
-      <c r="B20">
+      <c r="B20" s="4">
         <v>6315</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="4">
         <v>6313</v>
       </c>
-      <c r="D20">
+      <c r="D20" s="6">
         <v>6550</v>
       </c>
-      <c r="N20">
+      <c r="F20" s="14">
         <v>5471</v>
       </c>
-    </row>
-    <row r="21" spans="1:14">
-      <c r="A21">
+      <c r="G20" s="4"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="5">
         <v>6800</v>
       </c>
-      <c r="B21">
+      <c r="B21" s="4">
         <v>6571</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="4">
         <v>6560</v>
       </c>
-      <c r="D21">
+      <c r="D21" s="6">
         <v>6821</v>
       </c>
-      <c r="N21">
+      <c r="F21" s="14">
         <v>5520</v>
       </c>
-    </row>
-    <row r="22" spans="1:14">
-      <c r="A22">
+      <c r="G21" s="4"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="5">
         <v>6940</v>
       </c>
-      <c r="B22">
+      <c r="B22" s="4">
         <v>6840</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="4">
         <v>6383</v>
       </c>
-      <c r="D22">
+      <c r="D22" s="6">
         <v>8230</v>
       </c>
-      <c r="N22">
+      <c r="F22" s="14">
         <v>5740</v>
       </c>
-    </row>
-    <row r="23" spans="1:14">
-      <c r="A23">
+      <c r="G22" s="4"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="5">
         <v>8485</v>
       </c>
-      <c r="B23">
+      <c r="B23" s="4">
         <v>8480</v>
       </c>
-      <c r="C23">
+      <c r="C23" s="4">
         <v>8231</v>
       </c>
-      <c r="D23">
+      <c r="D23" s="6">
         <v>9000</v>
       </c>
-      <c r="N23">
+      <c r="F23" s="14">
         <v>7002</v>
       </c>
-    </row>
-    <row r="24" spans="1:14">
-      <c r="A24">
+      <c r="G23" s="4"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="5">
         <v>9041</v>
       </c>
-      <c r="B24">
+      <c r="B24" s="4">
         <v>9040</v>
       </c>
-      <c r="C24">
+      <c r="C24" s="4">
         <v>9001</v>
       </c>
-      <c r="D24">
+      <c r="D24" s="6">
         <v>9050</v>
       </c>
-      <c r="N24">
+      <c r="F24" s="14">
         <v>7004</v>
       </c>
-    </row>
-    <row r="25" spans="1:14">
-      <c r="A25">
+      <c r="G24" s="4"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="5">
         <v>9180</v>
       </c>
-      <c r="B25">
+      <c r="B25" s="4">
         <v>9140</v>
       </c>
-      <c r="C25">
+      <c r="C25" s="4">
         <v>9120</v>
       </c>
-      <c r="D25">
+      <c r="D25" s="6">
         <v>9181</v>
       </c>
-      <c r="N25">
+      <c r="F25" s="14">
         <v>7036</v>
       </c>
-    </row>
-    <row r="26" spans="1:14">
-      <c r="A26">
+      <c r="G25" s="4"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="5">
         <v>9230</v>
       </c>
-      <c r="B26">
+      <c r="B26" s="4">
         <v>9220</v>
       </c>
-      <c r="C26">
+      <c r="C26" s="4">
         <v>9210</v>
       </c>
-      <c r="D26">
+      <c r="D26" s="6">
         <v>9250</v>
       </c>
-      <c r="N26">
+      <c r="F26" s="14">
         <v>7037</v>
       </c>
-    </row>
-    <row r="27" spans="1:14">
-      <c r="A27">
+      <c r="G26" s="4"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="5">
         <v>9300</v>
       </c>
-      <c r="B27">
+      <c r="B27" s="4">
         <v>9270</v>
       </c>
-      <c r="C27">
+      <c r="C27" s="4">
         <v>9254</v>
       </c>
-      <c r="D27">
+      <c r="D27" s="6">
         <v>9301</v>
       </c>
-      <c r="N27">
+      <c r="F27" s="14">
         <v>7041</v>
       </c>
-    </row>
-    <row r="28" spans="1:14">
-      <c r="A28">
+      <c r="G27" s="4"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="5">
         <v>9340</v>
       </c>
-      <c r="B28">
+      <c r="B28" s="4">
         <v>9330</v>
       </c>
-      <c r="C28">
+      <c r="C28" s="4">
         <v>9320</v>
       </c>
-      <c r="D28">
+      <c r="D28" s="6">
         <v>9341</v>
       </c>
-      <c r="N28">
+      <c r="F28" s="14">
         <v>7130</v>
       </c>
-    </row>
-    <row r="29" spans="1:14">
-      <c r="A29">
+      <c r="G28" s="4"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="5">
         <v>9404</v>
       </c>
-      <c r="B29">
+      <c r="B29" s="4">
         <v>9373</v>
       </c>
-      <c r="C29">
+      <c r="C29" s="4">
         <v>9342</v>
       </c>
-      <c r="D29">
+      <c r="D29" s="6">
         <v>9405</v>
       </c>
-      <c r="N29">
+      <c r="F29" s="14">
         <v>7140</v>
       </c>
-    </row>
-    <row r="30" spans="1:14">
-      <c r="A30">
+      <c r="G29" s="4"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="5">
         <v>9410</v>
       </c>
-      <c r="B30">
+      <c r="B30" s="4">
         <v>9411</v>
       </c>
-      <c r="C30">
+      <c r="C30" s="4">
         <v>9409</v>
       </c>
-      <c r="D30">
+      <c r="D30" s="6">
         <v>9415</v>
       </c>
-      <c r="N30">
+      <c r="F30" s="14">
         <v>7205</v>
       </c>
-    </row>
-    <row r="31" spans="1:14">
-      <c r="A31">
+      <c r="G30" s="4"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="5">
         <v>9419</v>
       </c>
-      <c r="B31">
+      <c r="B31" s="4">
         <v>9420</v>
       </c>
-      <c r="C31">
+      <c r="C31" s="4">
         <v>9417</v>
       </c>
-      <c r="D31">
+      <c r="D31" s="6">
         <v>9421</v>
       </c>
-      <c r="N31">
+      <c r="F31" s="14">
         <v>7217</v>
       </c>
-    </row>
-    <row r="32" spans="1:14">
-      <c r="A32">
+      <c r="G31" s="4"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="5">
         <v>9425</v>
       </c>
-      <c r="B32">
+      <c r="B32" s="4">
         <v>9426</v>
       </c>
-      <c r="C32">
+      <c r="C32" s="4">
         <v>9423</v>
       </c>
-      <c r="D32">
+      <c r="D32" s="6">
         <v>9427</v>
       </c>
-      <c r="N32">
+      <c r="F32" s="14">
         <v>7491</v>
       </c>
-    </row>
-    <row r="33" spans="1:14">
-      <c r="A33">
+      <c r="G32" s="4"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="5">
         <v>9430</v>
       </c>
-      <c r="B33">
+      <c r="B33" s="4">
         <v>9440</v>
       </c>
-      <c r="C33">
+      <c r="C33" s="4">
         <v>9429</v>
       </c>
-      <c r="D33">
+      <c r="D33" s="6">
         <v>9452</v>
       </c>
-      <c r="N33">
+      <c r="F33" s="14">
         <v>7493</v>
       </c>
-    </row>
-    <row r="34" spans="1:14">
-      <c r="A34">
+      <c r="G33" s="4"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="5">
         <v>9471</v>
       </c>
-      <c r="B34">
+      <c r="B34" s="4">
         <v>9480</v>
       </c>
-      <c r="C34">
+      <c r="C34" s="4">
         <v>9470</v>
       </c>
-      <c r="D34">
+      <c r="D34" s="6">
         <v>9490</v>
       </c>
-      <c r="N34">
+      <c r="F34" s="14">
         <v>7495</v>
       </c>
-    </row>
-    <row r="35" spans="1:14">
-      <c r="A35">
+      <c r="G34" s="4"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="5">
         <v>9561</v>
       </c>
-      <c r="B35">
+      <c r="B35" s="4">
         <v>9570</v>
       </c>
-      <c r="C35">
+      <c r="C35" s="4">
         <v>9520</v>
       </c>
-      <c r="D35">
+      <c r="D35" s="6">
         <v>9571</v>
       </c>
-      <c r="N35">
+      <c r="F35" s="14">
         <v>7496</v>
       </c>
-    </row>
-    <row r="36" spans="1:14">
-      <c r="A36">
+      <c r="G35" s="4"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" s="5">
         <v>9584</v>
       </c>
-      <c r="B36">
+      <c r="B36" s="4">
         <v>9592</v>
       </c>
-      <c r="C36">
+      <c r="C36" s="4">
         <v>9582</v>
       </c>
-      <c r="D36">
+      <c r="D36" s="6">
         <v>9594</v>
       </c>
-      <c r="N36">
+      <c r="F36" s="14">
         <v>7504</v>
       </c>
-    </row>
-    <row r="37" spans="1:14">
-      <c r="A37">
+      <c r="G36" s="4"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" s="5">
         <v>9611</v>
       </c>
-      <c r="B37">
+      <c r="B37" s="4">
         <v>9620</v>
       </c>
-      <c r="C37">
+      <c r="C37" s="4">
         <v>9600</v>
       </c>
-      <c r="D37">
+      <c r="D37" s="6">
         <v>9622</v>
       </c>
-      <c r="N37">
+      <c r="F37" s="14">
         <v>7546</v>
       </c>
-    </row>
-    <row r="38" spans="1:14">
-      <c r="A38">
+      <c r="G37" s="4"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" s="5">
         <v>9635</v>
       </c>
-      <c r="B38">
+      <c r="B38" s="4">
         <v>9700</v>
       </c>
-      <c r="C38">
+      <c r="C38" s="4">
         <v>9630</v>
       </c>
-      <c r="D38">
+      <c r="D38" s="6">
         <v>9810</v>
       </c>
-      <c r="N38">
+      <c r="F38" s="14">
         <v>7550</v>
       </c>
-    </row>
-    <row r="39" spans="1:14">
-      <c r="A39">
+      <c r="G38" s="4"/>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" s="5">
         <v>9900</v>
       </c>
-      <c r="B39">
+      <c r="B39" s="4">
         <v>9901</v>
       </c>
-      <c r="C39">
+      <c r="C39" s="4">
         <v>9830</v>
       </c>
-      <c r="D39">
+      <c r="D39" s="6">
         <v>9902</v>
       </c>
-      <c r="N39">
+      <c r="F39" s="14">
         <v>7640</v>
       </c>
-    </row>
-    <row r="40" spans="1:14">
-      <c r="A40">
+      <c r="G39" s="4"/>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" s="5">
         <v>9910</v>
       </c>
-      <c r="B40">
+      <c r="B40" s="4">
         <v>9911</v>
       </c>
-      <c r="C40">
+      <c r="C40" s="4">
         <v>9903</v>
       </c>
-      <c r="D40">
+      <c r="D40" s="6">
         <v>9912</v>
       </c>
-      <c r="N40">
+      <c r="F40" s="14">
         <v>7705</v>
       </c>
-    </row>
-    <row r="41" spans="1:14">
-      <c r="A41" s="6">
+      <c r="G40" s="4"/>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" s="7">
         <v>9920</v>
       </c>
-      <c r="B41">
+      <c r="B41" s="8">
         <v>9921</v>
       </c>
-      <c r="C41">
+      <c r="C41" s="8">
         <v>9913</v>
       </c>
-      <c r="D41">
+      <c r="D41" s="3">
         <v>9925</v>
       </c>
-      <c r="N41">
+      <c r="F41" s="15">
         <v>8221</v>
       </c>
+      <c r="G41" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1550,15 +1679,15 @@
   <dimension ref="A1:K41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:C9"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="17.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -1566,7 +1695,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2272</v>
       </c>
@@ -1574,34 +1703,34 @@
         <v>1205</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D2">
         <v>1019</v>
       </c>
       <c r="E2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F2">
         <v>1022</v>
       </c>
       <c r="G2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H2">
         <v>1026</v>
       </c>
       <c r="I2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J2">
         <v>1030</v>
       </c>
       <c r="K2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2383</v>
       </c>
@@ -1609,34 +1738,34 @@
         <v>3103</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D3">
         <v>1040</v>
       </c>
       <c r="E3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F3">
         <v>1050</v>
       </c>
       <c r="G3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H3">
         <v>1051</v>
       </c>
       <c r="I3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J3">
         <v>1052</v>
       </c>
       <c r="K3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2393</v>
       </c>
@@ -1644,34 +1773,34 @@
         <v>3180</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D4">
         <v>1070</v>
       </c>
       <c r="E4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F4">
         <v>1080</v>
       </c>
       <c r="G4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H4">
         <v>1090</v>
       </c>
       <c r="I4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J4">
         <v>1101</v>
       </c>
       <c r="K4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2396</v>
       </c>
@@ -1679,34 +1808,34 @@
         <v>3213</v>
       </c>
       <c r="C5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D5">
         <v>1110</v>
       </c>
       <c r="E5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F5">
         <v>1111</v>
       </c>
       <c r="G5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H5">
         <v>1114</v>
       </c>
       <c r="I5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J5">
         <v>1200</v>
       </c>
       <c r="K5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2397</v>
       </c>
@@ -1714,34 +1843,34 @@
         <v>3220</v>
       </c>
       <c r="C6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D6">
         <v>1201</v>
       </c>
       <c r="E6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F6">
         <v>1274</v>
       </c>
       <c r="G6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H6">
         <v>1275</v>
       </c>
       <c r="I6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J6">
         <v>1300</v>
       </c>
       <c r="K6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2435</v>
       </c>
@@ -1749,34 +1878,34 @@
         <v>3280</v>
       </c>
       <c r="C7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D7">
         <v>1321</v>
       </c>
       <c r="E7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F7">
         <v>1302</v>
       </c>
       <c r="G7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H7">
         <v>1301</v>
       </c>
       <c r="I7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J7">
         <v>1932</v>
       </c>
       <c r="K7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2480</v>
       </c>
@@ -1784,34 +1913,34 @@
         <v>5970</v>
       </c>
       <c r="C8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D8">
         <v>2130</v>
       </c>
       <c r="E8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F8">
         <v>2120</v>
       </c>
       <c r="G8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H8">
         <v>2095</v>
       </c>
       <c r="I8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J8">
         <v>2205</v>
       </c>
       <c r="K8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2514</v>
       </c>
@@ -1819,34 +1948,34 @@
         <v>6190</v>
       </c>
       <c r="C9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D9">
         <v>2691</v>
       </c>
       <c r="E9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F9">
         <v>2683</v>
       </c>
       <c r="G9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H9">
         <v>2220</v>
       </c>
       <c r="I9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J9">
         <v>2692</v>
       </c>
       <c r="K9" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2518</v>
       </c>
@@ -1854,28 +1983,28 @@
         <v>2700</v>
       </c>
       <c r="E10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F10">
         <v>2695</v>
       </c>
       <c r="G10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H10">
         <v>2694</v>
       </c>
       <c r="I10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J10">
         <v>2703</v>
       </c>
       <c r="K10" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2575</v>
       </c>
@@ -1883,28 +2012,28 @@
         <v>2751</v>
       </c>
       <c r="E11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F11">
         <v>2705</v>
       </c>
       <c r="G11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H11">
         <v>2704</v>
       </c>
       <c r="I11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J11">
         <v>2795</v>
       </c>
       <c r="K11" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>2580</v>
       </c>
@@ -1912,28 +2041,28 @@
         <v>2811</v>
       </c>
       <c r="E12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F12">
         <v>2800</v>
       </c>
       <c r="G12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H12">
         <v>2799</v>
       </c>
       <c r="I12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J12">
         <v>2900</v>
       </c>
       <c r="K12" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2593</v>
       </c>
@@ -1941,28 +2070,28 @@
         <v>3016</v>
       </c>
       <c r="E13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F13">
         <v>3005</v>
       </c>
       <c r="G13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H13">
         <v>3001</v>
       </c>
       <c r="I13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J13">
         <v>3030</v>
       </c>
       <c r="K13" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2594</v>
       </c>
@@ -1970,28 +2099,28 @@
         <v>3215</v>
       </c>
       <c r="E14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F14">
         <v>3181</v>
       </c>
       <c r="G14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H14">
         <v>3110</v>
       </c>
       <c r="I14" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J14">
         <v>3225</v>
       </c>
       <c r="K14" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2870</v>
       </c>
@@ -1999,28 +2128,28 @@
         <v>3301</v>
       </c>
       <c r="E15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F15">
         <v>3300</v>
       </c>
       <c r="G15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H15">
         <v>3230</v>
       </c>
       <c r="I15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J15">
         <v>3500</v>
       </c>
       <c r="K15" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2880</v>
       </c>
@@ -2028,28 +2157,28 @@
         <v>5920</v>
       </c>
       <c r="E16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F16">
         <v>4621</v>
       </c>
       <c r="G16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H16">
         <v>3530</v>
       </c>
       <c r="I16" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="J16">
         <v>5950</v>
       </c>
       <c r="K16" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>2980</v>
       </c>
@@ -2057,28 +2186,28 @@
         <v>6010</v>
       </c>
       <c r="E17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F17">
         <v>5973</v>
       </c>
       <c r="G17" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H17">
         <v>5971</v>
       </c>
       <c r="I17" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J17">
         <v>6200</v>
       </c>
       <c r="K17" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>5395</v>
       </c>
@@ -2086,28 +2215,28 @@
         <v>6242</v>
       </c>
       <c r="E18" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F18">
         <v>6241</v>
       </c>
       <c r="G18" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H18">
         <v>6212</v>
       </c>
       <c r="I18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J18">
         <v>6243</v>
       </c>
       <c r="K18" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>5455</v>
       </c>
@@ -2115,28 +2244,28 @@
         <v>6311</v>
       </c>
       <c r="E19" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F19">
         <v>6260</v>
       </c>
       <c r="G19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H19">
         <v>6250</v>
       </c>
       <c r="I19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J19">
         <v>6312</v>
       </c>
       <c r="K19" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>5471</v>
       </c>
@@ -2144,28 +2273,28 @@
         <v>6370</v>
       </c>
       <c r="E20" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F20">
         <v>6315</v>
       </c>
       <c r="G20" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H20">
         <v>6313</v>
       </c>
       <c r="I20" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J20">
         <v>6550</v>
       </c>
       <c r="K20" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>5520</v>
       </c>
@@ -2173,28 +2302,28 @@
         <v>6800</v>
       </c>
       <c r="E21" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F21">
         <v>6571</v>
       </c>
       <c r="G21" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H21">
         <v>6560</v>
       </c>
       <c r="I21" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J21">
         <v>6821</v>
       </c>
       <c r="K21" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>5740</v>
       </c>
@@ -2202,28 +2331,28 @@
         <v>6940</v>
       </c>
       <c r="E22" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F22">
         <v>6840</v>
       </c>
       <c r="G22" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H22">
         <v>6383</v>
       </c>
       <c r="I22" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J22">
         <v>8230</v>
       </c>
       <c r="K22" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>7002</v>
       </c>
@@ -2231,28 +2360,28 @@
         <v>8485</v>
       </c>
       <c r="E23" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F23">
         <v>8480</v>
       </c>
       <c r="G23" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H23">
         <v>8231</v>
       </c>
       <c r="I23" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J23">
         <v>9000</v>
       </c>
       <c r="K23" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>7004</v>
       </c>
@@ -2260,28 +2389,28 @@
         <v>9041</v>
       </c>
       <c r="E24" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F24">
         <v>9040</v>
       </c>
       <c r="G24" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H24">
         <v>9001</v>
       </c>
       <c r="I24" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J24">
         <v>9050</v>
       </c>
       <c r="K24" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>7036</v>
       </c>
@@ -2289,28 +2418,28 @@
         <v>9180</v>
       </c>
       <c r="E25" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F25">
         <v>9140</v>
       </c>
       <c r="G25" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H25">
         <v>9120</v>
       </c>
       <c r="I25" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J25">
         <v>9181</v>
       </c>
       <c r="K25" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>7037</v>
       </c>
@@ -2318,28 +2447,28 @@
         <v>9230</v>
       </c>
       <c r="E26" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F26">
         <v>9220</v>
       </c>
       <c r="G26" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H26">
         <v>9210</v>
       </c>
       <c r="I26" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J26">
         <v>9250</v>
       </c>
       <c r="K26" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>7041</v>
       </c>
@@ -2347,28 +2476,28 @@
         <v>9300</v>
       </c>
       <c r="E27" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F27">
         <v>9270</v>
       </c>
       <c r="G27" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H27">
         <v>9254</v>
       </c>
       <c r="I27" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J27">
         <v>9301</v>
       </c>
       <c r="K27" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>7130</v>
       </c>
@@ -2376,28 +2505,28 @@
         <v>9340</v>
       </c>
       <c r="E28" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F28">
         <v>9330</v>
       </c>
       <c r="G28" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H28">
         <v>9320</v>
       </c>
       <c r="I28" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J28">
         <v>9341</v>
       </c>
       <c r="K28" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>7140</v>
       </c>
@@ -2405,28 +2534,28 @@
         <v>9404</v>
       </c>
       <c r="E29" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F29">
         <v>9373</v>
       </c>
       <c r="G29" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H29">
         <v>9342</v>
       </c>
       <c r="I29" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J29">
         <v>9405</v>
       </c>
       <c r="K29" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>7205</v>
       </c>
@@ -2434,28 +2563,28 @@
         <v>9410</v>
       </c>
       <c r="E30" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F30">
         <v>9411</v>
       </c>
       <c r="G30" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H30">
         <v>9409</v>
       </c>
       <c r="I30" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J30">
         <v>9415</v>
       </c>
       <c r="K30" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>7217</v>
       </c>
@@ -2463,28 +2592,28 @@
         <v>9419</v>
       </c>
       <c r="E31" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F31">
         <v>9420</v>
       </c>
       <c r="G31" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H31">
         <v>9417</v>
       </c>
       <c r="I31" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J31">
         <v>9421</v>
       </c>
       <c r="K31" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>7491</v>
       </c>
@@ -2492,28 +2621,28 @@
         <v>9425</v>
       </c>
       <c r="E32" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F32">
         <v>9426</v>
       </c>
       <c r="G32" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H32">
         <v>9423</v>
       </c>
       <c r="I32" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J32">
         <v>9427</v>
       </c>
       <c r="K32" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>7493</v>
       </c>
@@ -2521,28 +2650,28 @@
         <v>9430</v>
       </c>
       <c r="E33" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F33">
         <v>9440</v>
       </c>
       <c r="G33" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H33">
         <v>9429</v>
       </c>
       <c r="I33" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="J33">
         <v>9452</v>
       </c>
       <c r="K33" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>7495</v>
       </c>
@@ -2550,28 +2679,28 @@
         <v>9471</v>
       </c>
       <c r="E34" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F34">
         <v>9480</v>
       </c>
       <c r="G34" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H34">
         <v>9470</v>
       </c>
       <c r="I34" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J34">
         <v>9490</v>
       </c>
       <c r="K34" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>7496</v>
       </c>
@@ -2579,28 +2708,28 @@
         <v>9561</v>
       </c>
       <c r="E35" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F35">
         <v>9570</v>
       </c>
       <c r="G35" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H35">
         <v>9520</v>
       </c>
       <c r="I35" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="J35">
         <v>9571</v>
       </c>
       <c r="K35" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>7504</v>
       </c>
@@ -2608,28 +2737,28 @@
         <v>9584</v>
       </c>
       <c r="E36" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F36">
         <v>9592</v>
       </c>
       <c r="G36" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H36">
         <v>9582</v>
       </c>
       <c r="I36" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="J36">
         <v>9594</v>
       </c>
       <c r="K36" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>7546</v>
       </c>
@@ -2637,28 +2766,28 @@
         <v>9611</v>
       </c>
       <c r="E37" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F37">
         <v>9620</v>
       </c>
       <c r="G37" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H37">
         <v>9600</v>
       </c>
       <c r="I37" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="J37">
         <v>9622</v>
       </c>
       <c r="K37" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>7550</v>
       </c>
@@ -2666,28 +2795,28 @@
         <v>9635</v>
       </c>
       <c r="E38" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F38">
         <v>9700</v>
       </c>
       <c r="G38" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H38">
         <v>9630</v>
       </c>
       <c r="I38" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="J38">
         <v>9810</v>
       </c>
       <c r="K38" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>7640</v>
       </c>
@@ -2695,28 +2824,28 @@
         <v>9900</v>
       </c>
       <c r="E39" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F39">
         <v>9901</v>
       </c>
       <c r="G39" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H39">
         <v>9830</v>
       </c>
       <c r="I39" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="J39">
         <v>9902</v>
       </c>
       <c r="K39" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>7705</v>
       </c>
@@ -2724,28 +2853,28 @@
         <v>9910</v>
       </c>
       <c r="E40" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F40">
         <v>9911</v>
       </c>
       <c r="G40" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H40">
         <v>9903</v>
       </c>
       <c r="I40" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="J40">
         <v>9912</v>
       </c>
       <c r="K40" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>8221</v>
       </c>
@@ -2753,25 +2882,25 @@
         <v>9920</v>
       </c>
       <c r="E41" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F41">
         <v>9921</v>
       </c>
       <c r="G41" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H41">
         <v>9913</v>
       </c>
       <c r="I41" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="J41">
         <v>9925</v>
       </c>
       <c r="K41" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>